<commit_message>
FixBug 010 + Code 008
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM010労働保険事業所の登録.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM010労働保険事業所の登録.xlsx
@@ -859,16 +859,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -45033,8 +45033,8 @@
       <c r="D2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="31"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="29"/>
       <c r="G2" s="16" t="s">
         <v>16</v>
       </c>
@@ -45048,8 +45048,8 @@
       <c r="D3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="29"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="31"/>
       <c r="G3" s="17" t="s">
         <v>17</v>
       </c>
@@ -45119,8 +45119,8 @@
       <c r="D10" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="31"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="29"/>
       <c r="G10" s="16" t="s">
         <v>10</v>
       </c>
@@ -45134,8 +45134,8 @@
       <c r="D11" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="28"/>
-      <c r="F11" s="29"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="31"/>
       <c r="G11" s="17" t="s">
         <v>2</v>
       </c>

</xml_diff>